<commit_message>
Progressing Anvanced Company Search function in Web Office, Also created Primary Test Suites for 3 Environments, Live, Dev and Preview
</commit_message>
<xml_diff>
--- a/Data Files/Advanced_Company_Search_Data.xlsx
+++ b/Data Files/Advanced_Company_Search_Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\davidho\Katalon Studio\Start\Data Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABE1B78A-F38E-48BE-9D27-D76E758D5838}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6838FA8A-859E-4C93-8B63-4D8EB1501332}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="29430" yWindow="1560" windowWidth="21600" windowHeight="11145" xr2:uid="{649E12C2-AF46-45B2-BAEF-B452665C1479}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{649E12C2-AF46-45B2-BAEF-B452665C1479}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="117">
   <si>
     <t>Trader_ID</t>
   </si>
@@ -90,6 +90,300 @@
   </si>
   <si>
     <t>Case_More_Than</t>
+  </si>
+  <si>
+    <t>Non_Member</t>
+  </si>
+  <si>
+    <t>Member</t>
+  </si>
+  <si>
+    <t>Both_Members_Non_Members</t>
+  </si>
+  <si>
+    <t>Exclude_Ex_Members</t>
+  </si>
+  <si>
+    <t>membership_Level</t>
+  </si>
+  <si>
+    <t>Fees_Both_Types</t>
+  </si>
+  <si>
+    <t>Fees_None</t>
+  </si>
+  <si>
+    <t>Fees_paying</t>
+  </si>
+  <si>
+    <t>Exclude_Duplicates</t>
+  </si>
+  <si>
+    <t>Marketing_Source_LB</t>
+  </si>
+  <si>
+    <t>Join_Reason_LB</t>
+  </si>
+  <si>
+    <t>Payment_Status_LB</t>
+  </si>
+  <si>
+    <t>Accreditation_Type_LB</t>
+  </si>
+  <si>
+    <t>Marketing_Type_LB</t>
+  </si>
+  <si>
+    <t>Marketing_Region_LB</t>
+  </si>
+  <si>
+    <t>ost_Email_LB</t>
+  </si>
+  <si>
+    <t>ost_Mobile_LB</t>
+  </si>
+  <si>
+    <t>ost_CAT_Insurance_LB</t>
+  </si>
+  <si>
+    <t>ost_Employees</t>
+  </si>
+  <si>
+    <t>ost_Show_Only_LB</t>
+  </si>
+  <si>
+    <t>tsic_Office_LB</t>
+  </si>
+  <si>
+    <t>tsic_Outcome_CB</t>
+  </si>
+  <si>
+    <t>tsic_OutcomeRB</t>
+  </si>
+  <si>
+    <t>EXPIRATIONS_TD</t>
+  </si>
+  <si>
+    <t>Public_Liability_RB</t>
+  </si>
+  <si>
+    <t>Public_Liability_CB</t>
+  </si>
+  <si>
+    <t>pl_Start_Date</t>
+  </si>
+  <si>
+    <t>pl_End_Date</t>
+  </si>
+  <si>
+    <t>Recommendations_RB</t>
+  </si>
+  <si>
+    <t>Recommendations_CB</t>
+  </si>
+  <si>
+    <t>Rec_Start_Date</t>
+  </si>
+  <si>
+    <t>Rec_End_Date</t>
+  </si>
+  <si>
+    <t>Recommend_Letter_RB</t>
+  </si>
+  <si>
+    <t>Recommend_Letter_CB</t>
+  </si>
+  <si>
+    <t>RecLet_Start_Date</t>
+  </si>
+  <si>
+    <t>RecLet_End_Date</t>
+  </si>
+  <si>
+    <t>Address_Complet_RB</t>
+  </si>
+  <si>
+    <t>Website_Live_RB</t>
+  </si>
+  <si>
+    <t>Hidden_From_Searches_RB</t>
+  </si>
+  <si>
+    <t>hfs_Not_Specified_CB</t>
+  </si>
+  <si>
+    <t>hfs_Public_Liability_Expired_CB</t>
+  </si>
+  <si>
+    <t>Address_Verification_CB</t>
+  </si>
+  <si>
+    <t>hfs_Accreditation_Expired_CB</t>
+  </si>
+  <si>
+    <t>Affiliate_Member_CB</t>
+  </si>
+  <si>
+    <t>Change_of_Company_Details_CB</t>
+  </si>
+  <si>
+    <t>hfs_Other_CB</t>
+  </si>
+  <si>
+    <t>hfs_Too_Much_Work_CB</t>
+  </si>
+  <si>
+    <t>Monitor_Reports_CB</t>
+  </si>
+  <si>
+    <t>mr_Less_LB</t>
+  </si>
+  <si>
+    <t>mr_Than_tb</t>
+  </si>
+  <si>
+    <t>mr_Since_Date</t>
+  </si>
+  <si>
+    <t>Vetting_Referrences_LB</t>
+  </si>
+  <si>
+    <t>vr_Less_Tahn_TB</t>
+  </si>
+  <si>
+    <t>Complaint_Status_LB</t>
+  </si>
+  <si>
+    <t>Complaint_Status_CB</t>
+  </si>
+  <si>
+    <t>Privacy_CB</t>
+  </si>
+  <si>
+    <t>Privacy_Share_Data_LB</t>
+  </si>
+  <si>
+    <t>tps_SMS_RB</t>
+  </si>
+  <si>
+    <t>tps_Phone_RB</t>
+  </si>
+  <si>
+    <t>tps_Email_RB</t>
+  </si>
+  <si>
+    <t>tps_Post</t>
+  </si>
+  <si>
+    <t>Lead_Type_CB</t>
+  </si>
+  <si>
+    <t>Lead_Type_LB</t>
+  </si>
+  <si>
+    <t>Company_Records_Creation_Date_CB</t>
+  </si>
+  <si>
+    <t>Company_Records_Creation_Date_Between</t>
+  </si>
+  <si>
+    <t>Company_Records_Creation_Date_Final</t>
+  </si>
+  <si>
+    <t>Paper_Invoicing_CB</t>
+  </si>
+  <si>
+    <t>Paper_Invoicing_RB</t>
+  </si>
+  <si>
+    <t>Classification_LB</t>
+  </si>
+  <si>
+    <t>Partner_Franchise_LB</t>
+  </si>
+  <si>
+    <t>Company_Name</t>
+  </si>
+  <si>
+    <t>Company_Alias</t>
+  </si>
+  <si>
+    <t>Directory_Heading_LB</t>
+  </si>
+  <si>
+    <t>Owner_Surname</t>
+  </si>
+  <si>
+    <t>Owner_DOB_CB</t>
+  </si>
+  <si>
+    <t>Owner_DOB</t>
+  </si>
+  <si>
+    <t>Name_House</t>
+  </si>
+  <si>
+    <t>Number_Street</t>
+  </si>
+  <si>
+    <t>Town</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>County</t>
+  </si>
+  <si>
+    <t>Postcode</t>
+  </si>
+  <si>
+    <t>Tel</t>
+  </si>
+  <si>
+    <t>Secure_Number</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Website</t>
+  </si>
+  <si>
+    <t>Show_Record_Count_CB</t>
+  </si>
+  <si>
+    <t>Primary_Web_Category_LB</t>
+  </si>
+  <si>
+    <t>PWC_RB</t>
+  </si>
+  <si>
+    <t>Secondary_Web_Category_LB</t>
+  </si>
+  <si>
+    <t>SWC_RB</t>
+  </si>
+  <si>
+    <t>Search_Mode_RB</t>
+  </si>
+  <si>
+    <t>true</t>
+  </si>
+  <si>
+    <t>22/01/1970</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>returns 4 records as of 22/01/2020 - IDs - 125227,215677,262755,460559</t>
+  </si>
+  <si>
+    <t>215677</t>
+  </si>
+  <si>
+    <t>Crystal Clear Ovens</t>
   </si>
 </sst>
 </file>
@@ -125,8 +419,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -441,19 +736,122 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD632F13-A4DF-4061-B337-99CDBF2689E4}">
-  <dimension ref="A1:S1"/>
+  <dimension ref="A1:DH21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="T1" sqref="T1"/>
+    <sheetView tabSelected="1" topLeftCell="CS1" workbookViewId="0">
+      <selection activeCell="DH3" sqref="DH3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.42578125" customWidth="1"/>
-    <col min="2" max="2" width="24.7109375" customWidth="1"/>
+    <col min="2" max="2" width="27.5703125" customWidth="1"/>
+    <col min="5" max="5" width="17.7109375" customWidth="1"/>
+    <col min="7" max="7" width="15.140625" customWidth="1"/>
+    <col min="8" max="8" width="17.85546875" customWidth="1"/>
+    <col min="9" max="9" width="21" customWidth="1"/>
+    <col min="10" max="10" width="15.5703125" customWidth="1"/>
+    <col min="11" max="12" width="17.28515625" customWidth="1"/>
+    <col min="13" max="13" width="26.42578125" customWidth="1"/>
+    <col min="14" max="14" width="20" customWidth="1"/>
+    <col min="15" max="15" width="19" customWidth="1"/>
+    <col min="16" max="16" width="23.140625" customWidth="1"/>
+    <col min="17" max="17" width="17.5703125" customWidth="1"/>
+    <col min="18" max="18" width="21.85546875" customWidth="1"/>
+    <col min="19" max="19" width="16.5703125" customWidth="1"/>
+    <col min="20" max="20" width="13.7109375" customWidth="1"/>
+    <col min="21" max="21" width="10.28515625" customWidth="1"/>
+    <col min="22" max="22" width="29.5703125" customWidth="1"/>
+    <col min="23" max="23" width="20.85546875" customWidth="1"/>
+    <col min="24" max="24" width="18.140625" customWidth="1"/>
+    <col min="25" max="25" width="15.42578125" customWidth="1"/>
+    <col min="26" max="26" width="13" customWidth="1"/>
+    <col min="27" max="27" width="12.85546875" customWidth="1"/>
+    <col min="28" max="28" width="18.5703125" customWidth="1"/>
+    <col min="29" max="29" width="19.5703125" customWidth="1"/>
+    <col min="30" max="30" width="14.85546875" customWidth="1"/>
+    <col min="31" max="31" width="15.28515625" customWidth="1"/>
+    <col min="32" max="32" width="18" customWidth="1"/>
+    <col min="33" max="33" width="15" customWidth="1"/>
+    <col min="34" max="34" width="16.85546875" customWidth="1"/>
+    <col min="35" max="35" width="13.85546875" customWidth="1"/>
+    <col min="36" max="36" width="14.28515625" customWidth="1"/>
+    <col min="37" max="37" width="15.42578125" customWidth="1"/>
+    <col min="38" max="38" width="14.7109375" customWidth="1"/>
+    <col min="39" max="39" width="17.42578125" customWidth="1"/>
+    <col min="40" max="40" width="13.42578125" customWidth="1"/>
+    <col min="41" max="42" width="16.140625" customWidth="1"/>
+    <col min="43" max="43" width="16" customWidth="1"/>
+    <col min="44" max="44" width="18.42578125" customWidth="1"/>
+    <col min="45" max="45" width="17" customWidth="1"/>
+    <col min="46" max="46" width="13.42578125" customWidth="1"/>
+    <col min="47" max="47" width="12.140625" customWidth="1"/>
+    <col min="48" max="48" width="16.140625" customWidth="1"/>
+    <col min="49" max="49" width="16.28515625" customWidth="1"/>
+    <col min="50" max="50" width="15" customWidth="1"/>
+    <col min="51" max="51" width="16.140625" customWidth="1"/>
+    <col min="52" max="53" width="14.42578125" customWidth="1"/>
+    <col min="54" max="54" width="17" customWidth="1"/>
+    <col min="55" max="55" width="16.28515625" customWidth="1"/>
+    <col min="56" max="56" width="18" customWidth="1"/>
+    <col min="57" max="57" width="17.28515625" customWidth="1"/>
+    <col min="58" max="58" width="25" customWidth="1"/>
+    <col min="59" max="59" width="21" customWidth="1"/>
+    <col min="60" max="60" width="27" customWidth="1"/>
+    <col min="61" max="61" width="23.28515625" customWidth="1"/>
+    <col min="62" max="62" width="29.140625" customWidth="1"/>
+    <col min="63" max="63" width="20.28515625" customWidth="1"/>
+    <col min="64" max="64" width="26.7109375" customWidth="1"/>
+    <col min="65" max="65" width="13.5703125" customWidth="1"/>
+    <col min="66" max="66" width="23" customWidth="1"/>
+    <col min="67" max="67" width="19.85546875" customWidth="1"/>
+    <col min="68" max="68" width="11.28515625" customWidth="1"/>
+    <col min="69" max="69" width="11.5703125" customWidth="1"/>
+    <col min="70" max="70" width="14.42578125" customWidth="1"/>
+    <col min="71" max="71" width="22.7109375" customWidth="1"/>
+    <col min="72" max="72" width="15.85546875" customWidth="1"/>
+    <col min="73" max="73" width="20.140625" customWidth="1"/>
+    <col min="74" max="74" width="21" customWidth="1"/>
+    <col min="75" max="75" width="11.85546875" customWidth="1"/>
+    <col min="76" max="76" width="22.28515625" customWidth="1"/>
+    <col min="77" max="77" width="12.28515625" customWidth="1"/>
+    <col min="78" max="78" width="14" customWidth="1"/>
+    <col min="79" max="79" width="13" customWidth="1"/>
+    <col min="80" max="80" width="8.5703125" customWidth="1"/>
+    <col min="81" max="81" width="14.28515625" customWidth="1"/>
+    <col min="82" max="82" width="13.7109375" customWidth="1"/>
+    <col min="83" max="83" width="35.140625" customWidth="1"/>
+    <col min="84" max="84" width="31.7109375" customWidth="1"/>
+    <col min="85" max="85" width="34.5703125" customWidth="1"/>
+    <col min="86" max="86" width="18.85546875" customWidth="1"/>
+    <col min="87" max="87" width="19.28515625" customWidth="1"/>
+    <col min="88" max="88" width="16" customWidth="1"/>
+    <col min="89" max="89" width="20.85546875" customWidth="1"/>
+    <col min="90" max="90" width="15.7109375" customWidth="1"/>
+    <col min="91" max="91" width="15.140625" customWidth="1"/>
+    <col min="92" max="92" width="21.85546875" customWidth="1"/>
+    <col min="93" max="93" width="15.5703125" customWidth="1"/>
+    <col min="94" max="94" width="17.42578125" customWidth="1"/>
+    <col min="95" max="95" width="16.140625" customWidth="1"/>
+    <col min="96" max="96" width="15.42578125" customWidth="1"/>
+    <col min="97" max="97" width="17.28515625" customWidth="1"/>
+    <col min="98" max="98" width="7.28515625" customWidth="1"/>
+    <col min="99" max="99" width="6.42578125" customWidth="1"/>
+    <col min="100" max="100" width="7.28515625" customWidth="1"/>
+    <col min="102" max="102" width="5" customWidth="1"/>
+    <col min="103" max="103" width="15.140625" customWidth="1"/>
+    <col min="104" max="104" width="7" customWidth="1"/>
+    <col min="105" max="105" width="12.28515625" customWidth="1"/>
+    <col min="106" max="106" width="23.42578125" customWidth="1"/>
+    <col min="107" max="107" width="24.5703125" customWidth="1"/>
+    <col min="108" max="108" width="13.42578125" customWidth="1"/>
+    <col min="109" max="109" width="23.85546875" customWidth="1"/>
+    <col min="110" max="110" width="13.7109375" customWidth="1"/>
+    <col min="111" max="111" width="14.85546875" customWidth="1"/>
+    <col min="112" max="112" width="54.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:112" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -511,8 +909,325 @@
       <c r="S1" t="s">
         <v>18</v>
       </c>
+      <c r="T1" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" t="s">
+        <v>22</v>
+      </c>
+      <c r="X1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AK1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AL1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AM1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AN1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AO1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AP1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AQ1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AR1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AS1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AT1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AU1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AV1" t="s">
+        <v>47</v>
+      </c>
+      <c r="AW1" t="s">
+        <v>48</v>
+      </c>
+      <c r="AX1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AY1" t="s">
+        <v>50</v>
+      </c>
+      <c r="AZ1" t="s">
+        <v>51</v>
+      </c>
+      <c r="BA1" t="s">
+        <v>52</v>
+      </c>
+      <c r="BB1" t="s">
+        <v>53</v>
+      </c>
+      <c r="BC1" t="s">
+        <v>54</v>
+      </c>
+      <c r="BD1" t="s">
+        <v>55</v>
+      </c>
+      <c r="BE1" t="s">
+        <v>56</v>
+      </c>
+      <c r="BF1" t="s">
+        <v>57</v>
+      </c>
+      <c r="BG1" t="s">
+        <v>58</v>
+      </c>
+      <c r="BH1" t="s">
+        <v>59</v>
+      </c>
+      <c r="BI1" t="s">
+        <v>60</v>
+      </c>
+      <c r="BJ1" t="s">
+        <v>61</v>
+      </c>
+      <c r="BK1" t="s">
+        <v>62</v>
+      </c>
+      <c r="BL1" t="s">
+        <v>63</v>
+      </c>
+      <c r="BM1" t="s">
+        <v>64</v>
+      </c>
+      <c r="BN1" t="s">
+        <v>65</v>
+      </c>
+      <c r="BO1" t="s">
+        <v>66</v>
+      </c>
+      <c r="BP1" t="s">
+        <v>67</v>
+      </c>
+      <c r="BQ1" t="s">
+        <v>68</v>
+      </c>
+      <c r="BR1" t="s">
+        <v>69</v>
+      </c>
+      <c r="BS1" t="s">
+        <v>70</v>
+      </c>
+      <c r="BT1" t="s">
+        <v>71</v>
+      </c>
+      <c r="BU1" t="s">
+        <v>73</v>
+      </c>
+      <c r="BV1" t="s">
+        <v>72</v>
+      </c>
+      <c r="BW1" t="s">
+        <v>74</v>
+      </c>
+      <c r="BX1" t="s">
+        <v>75</v>
+      </c>
+      <c r="BY1" t="s">
+        <v>76</v>
+      </c>
+      <c r="BZ1" t="s">
+        <v>77</v>
+      </c>
+      <c r="CA1" t="s">
+        <v>78</v>
+      </c>
+      <c r="CB1" t="s">
+        <v>79</v>
+      </c>
+      <c r="CC1" t="s">
+        <v>80</v>
+      </c>
+      <c r="CD1" t="s">
+        <v>81</v>
+      </c>
+      <c r="CE1" t="s">
+        <v>82</v>
+      </c>
+      <c r="CF1" t="s">
+        <v>83</v>
+      </c>
+      <c r="CG1" t="s">
+        <v>84</v>
+      </c>
+      <c r="CH1" t="s">
+        <v>85</v>
+      </c>
+      <c r="CI1" t="s">
+        <v>86</v>
+      </c>
+      <c r="CJ1" t="s">
+        <v>87</v>
+      </c>
+      <c r="CK1" t="s">
+        <v>88</v>
+      </c>
+      <c r="CL1" t="s">
+        <v>89</v>
+      </c>
+      <c r="CM1" t="s">
+        <v>90</v>
+      </c>
+      <c r="CN1" t="s">
+        <v>91</v>
+      </c>
+      <c r="CO1" t="s">
+        <v>92</v>
+      </c>
+      <c r="CP1" t="s">
+        <v>93</v>
+      </c>
+      <c r="CQ1" t="s">
+        <v>94</v>
+      </c>
+      <c r="CR1" t="s">
+        <v>95</v>
+      </c>
+      <c r="CS1" t="s">
+        <v>96</v>
+      </c>
+      <c r="CT1" t="s">
+        <v>97</v>
+      </c>
+      <c r="CU1" t="s">
+        <v>98</v>
+      </c>
+      <c r="CV1" t="s">
+        <v>99</v>
+      </c>
+      <c r="CW1" t="s">
+        <v>100</v>
+      </c>
+      <c r="CX1" t="s">
+        <v>101</v>
+      </c>
+      <c r="CY1" t="s">
+        <v>102</v>
+      </c>
+      <c r="CZ1" t="s">
+        <v>103</v>
+      </c>
+      <c r="DA1" t="s">
+        <v>104</v>
+      </c>
+      <c r="DB1" t="s">
+        <v>105</v>
+      </c>
+      <c r="DC1" t="s">
+        <v>106</v>
+      </c>
+      <c r="DD1" t="s">
+        <v>107</v>
+      </c>
+      <c r="DE1" t="s">
+        <v>108</v>
+      </c>
+      <c r="DF1" t="s">
+        <v>109</v>
+      </c>
+      <c r="DG1" t="s">
+        <v>110</v>
+      </c>
+      <c r="DH1" t="s">
+        <v>113</v>
+      </c>
     </row>
+    <row r="2" spans="1:112" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="CP2" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="CQ2" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="DH2" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="3" spans="1:112" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="DH3" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="4" spans="1:112" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="1:112" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="1:112" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="1:112" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="1:112" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:112" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="1:112" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:112" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:112" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:112" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:112" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:112" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:112" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="17" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="18" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="19" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="20" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="21" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Advanced WO Search Company Datafile update
</commit_message>
<xml_diff>
--- a/Data Files/Advanced_Company_Search_Data.xlsx
+++ b/Data Files/Advanced_Company_Search_Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\davidho\Katalon Studio\Start\Data Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6838FA8A-859E-4C93-8B63-4D8EB1501332}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60E3C016-16DF-48BD-A244-8FAA1215CB4E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{649E12C2-AF46-45B2-BAEF-B452665C1479}"/>
+    <workbookView minimized="1" xWindow="11355" yWindow="1620" windowWidth="10260" windowHeight="5580" xr2:uid="{649E12C2-AF46-45B2-BAEF-B452665C1479}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="143">
   <si>
     <t>Trader_ID</t>
   </si>
@@ -371,32 +371,129 @@
     <t>true</t>
   </si>
   <si>
-    <t>22/01/1970</t>
-  </si>
-  <si>
     <t>Comments</t>
   </si>
   <si>
-    <t>returns 4 records as of 22/01/2020 - IDs - 125227,215677,262755,460559</t>
-  </si>
-  <si>
-    <t>215677</t>
-  </si>
-  <si>
-    <t>Crystal Clear Ovens</t>
+    <t>280592</t>
+  </si>
+  <si>
+    <t>gordon@drainboss.co.uk</t>
+  </si>
+  <si>
+    <t>2 Redwood Drive</t>
+  </si>
+  <si>
+    <t>Haywards Heath</t>
+  </si>
+  <si>
+    <t>West Sussex</t>
+  </si>
+  <si>
+    <t>RH16 4ER</t>
+  </si>
+  <si>
+    <t>01444 657789</t>
+  </si>
+  <si>
+    <t>Brown</t>
+  </si>
+  <si>
+    <t>Page_Header_Text</t>
+  </si>
+  <si>
+    <t>BLOCKED DRAINS</t>
+  </si>
+  <si>
+    <t>Full_Name</t>
+  </si>
+  <si>
+    <t>Full_Address</t>
+  </si>
+  <si>
+    <t>2 Redwood Drive, Haywards Heath, West Sussex, RH16 4ER</t>
+  </si>
+  <si>
+    <t>Mr Gordon Brown</t>
+  </si>
+  <si>
+    <t>DoB: 23/01/1967</t>
+  </si>
+  <si>
+    <t>Checkatrade.com/BlockedDrains</t>
+  </si>
+  <si>
+    <t>DoB: 18/09/1959</t>
+  </si>
+  <si>
+    <t>kfrsteve@hotmail.com</t>
+  </si>
+  <si>
+    <t>01243 868423</t>
+  </si>
+  <si>
+    <t>Lyndale, Town Cross Avenue, Bognor Regis, West Sussex, PO21 2DN</t>
+  </si>
+  <si>
+    <t>Kitchen Facelift &amp; Renewal Limited</t>
+  </si>
+  <si>
+    <t>Mr Steve Mercer</t>
+  </si>
+  <si>
+    <t>Lots of detail set to search for Regular Trader, Returned Checked</t>
+  </si>
+  <si>
+    <t>Trader ID Only set to search for Regular Trader, Returned Checked</t>
+  </si>
+  <si>
+    <t>limited Company Number Search Only set to search for Ltd Co Trader, Returned Checked</t>
+  </si>
+  <si>
+    <t>Lots of detail set to search for Limited Company, Returned Checked</t>
+  </si>
+  <si>
+    <t>Symes Garden Services</t>
+  </si>
+  <si>
+    <t>Mr Bob Symes</t>
+  </si>
+  <si>
+    <t>3 digit trader ID search, verify returnes</t>
+  </si>
+  <si>
+    <t>8 The Newlands, Wallington, Greater London, SM6 9JU</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF555555"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF555555"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF666666"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -419,9 +516,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -736,10 +842,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD632F13-A4DF-4061-B337-99CDBF2689E4}">
-  <dimension ref="A1:DH21"/>
+  <dimension ref="A1:DK6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="CS1" workbookViewId="0">
-      <selection activeCell="DH3" sqref="DH3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7:XFD18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -834,24 +940,25 @@
     <col min="94" max="94" width="17.42578125" customWidth="1"/>
     <col min="95" max="95" width="16.140625" customWidth="1"/>
     <col min="96" max="96" width="15.42578125" customWidth="1"/>
-    <col min="97" max="97" width="17.28515625" customWidth="1"/>
-    <col min="98" max="98" width="7.28515625" customWidth="1"/>
-    <col min="99" max="99" width="6.42578125" customWidth="1"/>
-    <col min="100" max="100" width="7.28515625" customWidth="1"/>
-    <col min="102" max="102" width="5" customWidth="1"/>
-    <col min="103" max="103" width="15.140625" customWidth="1"/>
-    <col min="104" max="104" width="7" customWidth="1"/>
-    <col min="105" max="105" width="12.28515625" customWidth="1"/>
+    <col min="97" max="97" width="26.85546875" customWidth="1"/>
+    <col min="98" max="98" width="11.140625" customWidth="1"/>
+    <col min="99" max="99" width="17.28515625" customWidth="1"/>
+    <col min="100" max="100" width="13.140625" customWidth="1"/>
+    <col min="101" max="101" width="15.28515625" customWidth="1"/>
+    <col min="102" max="103" width="24" customWidth="1"/>
+    <col min="104" max="104" width="22.42578125" customWidth="1"/>
+    <col min="105" max="105" width="23.85546875" customWidth="1"/>
     <col min="106" max="106" width="23.42578125" customWidth="1"/>
     <col min="107" max="107" width="24.5703125" customWidth="1"/>
     <col min="108" max="108" width="13.42578125" customWidth="1"/>
     <col min="109" max="109" width="23.85546875" customWidth="1"/>
     <col min="110" max="110" width="13.7109375" customWidth="1"/>
-    <col min="111" max="111" width="14.85546875" customWidth="1"/>
-    <col min="112" max="112" width="54.85546875" customWidth="1"/>
+    <col min="111" max="113" width="26" customWidth="1"/>
+    <col min="114" max="114" width="35" customWidth="1"/>
+    <col min="115" max="115" width="54.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:112" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:115" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1183,49 +1290,145 @@
         <v>109</v>
       </c>
       <c r="DG1" t="s">
+        <v>121</v>
+      </c>
+      <c r="DH1" t="s">
+        <v>123</v>
+      </c>
+      <c r="DI1" t="s">
+        <v>124</v>
+      </c>
+      <c r="DJ1" t="s">
         <v>110</v>
       </c>
-      <c r="DH1" t="s">
+      <c r="DK1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="2" spans="1:115" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="2" spans="1:112" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="CO2" s="1" t="s">
+        <v>120</v>
+      </c>
       <c r="CP2" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="CQ2" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="DH2" s="1" t="s">
+      <c r="CQ2" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="CS2" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="CU2" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="CV2" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="CW2" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="CX2" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="CZ2" s="2" t="s">
         <v>114</v>
       </c>
+      <c r="DA2" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="DG2" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="DH2" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="DI2" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="DK2" s="1" t="s">
+        <v>135</v>
+      </c>
     </row>
-    <row r="3" spans="1:112" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:115" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="DH3" s="1" t="s">
-        <v>116</v>
+        <v>113</v>
+      </c>
+      <c r="DG3" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="DH3" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="DI3" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="DK3" s="1" t="s">
+        <v>136</v>
       </c>
     </row>
-    <row r="4" spans="1:112" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="1:112" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="6" spans="1:112" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="1:112" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="8" spans="1:112" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="9" spans="1:112" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="1:112" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="1:112" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="1:112" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="1:112" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="1:112" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="1:112" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="1:112" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="17" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="18" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="19" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="20" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="21" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="1:115" x14ac:dyDescent="0.25">
+      <c r="B4" s="5">
+        <v>4460222</v>
+      </c>
+      <c r="CQ4" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="CX4" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="CZ4" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="DG4" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="DH4" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="DI4" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="DK4" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="5" spans="1:115" x14ac:dyDescent="0.25">
+      <c r="B5" s="5">
+        <v>4460222</v>
+      </c>
+      <c r="DG5" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="DH5" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="DI5" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="DK5" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="6" spans="1:115" x14ac:dyDescent="0.25">
+      <c r="A6" s="6">
+        <v>105</v>
+      </c>
+      <c r="DG6" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="DH6" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="DI6" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="DK6" s="1" t="s">
+        <v>141</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>